<commit_message>
Kiem thu Hino 1
</commit_message>
<xml_diff>
--- a/demo13_Selenium_ReportTest/Resources/data/test-login.xlsx
+++ b/demo13_Selenium_ReportTest/Resources/data/test-login.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>STT</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -402,10 +405,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -413,5 +416,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>